<commit_message>
Backup folder - 2023-12-20 21:09:38
</commit_message>
<xml_diff>
--- a/АСД/РР1/Все в одному+гарні графіки.xlsx
+++ b/АСД/РР1/Все в одному+гарні графіки.xlsx
@@ -8,31 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yarik/Desktop/✈️ ХАІ 💻/АСД/РР1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D340E396-7928-094A-BEEF-42B8E1F6EBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6305A563-BF06-7749-BDCA-8CFABC0E63C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="5320" windowWidth="17460" windowHeight="12200" activeTab="2" xr2:uid="{1A0BFC92-E664-0641-8C63-6A9B31C871B1}"/>
+    <workbookView xWindow="520" yWindow="1520" windowWidth="14240" windowHeight="15860" activeTab="2" xr2:uid="{1A0BFC92-E664-0641-8C63-6A9B31C871B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Додавання" sheetId="1" r:id="rId1"/>
     <sheet name="Видалення" sheetId="2" r:id="rId2"/>
     <sheet name="Сортування" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Сортування!$A$2</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Сортування!$A$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Сортування!$A$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Сортування!$B$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Сортування!$B$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Сортування!$B$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Сортування!$B$4:$G$4</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Сортування!$B$1:$G$1</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Сортування!$B$2:$G$2</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Сортування!$B$3:$G$3</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Сортування!$B$4:$G$4</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">Сортування!$A$2</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">Сортування!$A$3</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">Сортування!$A$4</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -110,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,14 +122,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -283,6 +259,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,25 +289,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3963,7 +3942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE0E456-CB31-F645-860B-C3D2922F1515}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -4070,21 +4049,21 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
@@ -4099,7 +4078,7 @@
       <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="10">
         <v>10000</v>
       </c>
       <c r="C13" s="1">
@@ -4116,7 +4095,7 @@
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="1">
         <v>15613</v>
       </c>
@@ -4131,7 +4110,7 @@
       <c r="A15" s="7">
         <v>3</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="10">
         <v>50000</v>
       </c>
       <c r="C15" s="1">
@@ -4148,7 +4127,7 @@
       <c r="A16" s="7">
         <v>4</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="1">
         <v>94982</v>
       </c>
@@ -4163,7 +4142,7 @@
       <c r="A17" s="7">
         <v>5</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="10">
         <v>100000</v>
       </c>
       <c r="C17" s="1">
@@ -4180,7 +4159,7 @@
       <c r="A18" s="7">
         <v>6</v>
       </c>
-      <c r="B18" s="17"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1">
         <v>585621</v>
       </c>
@@ -4211,7 +4190,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C16" sqref="C16:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4319,21 +4298,21 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="6" t="s">
         <v>3</v>
       </c>
@@ -4348,7 +4327,7 @@
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="22">
         <v>10000</v>
       </c>
       <c r="C16" s="1">
@@ -4365,9 +4344,7 @@
       <c r="A17" s="7">
         <v>2</v>
       </c>
-      <c r="B17" s="18">
-        <v>10000</v>
-      </c>
+      <c r="B17" s="23"/>
       <c r="C17" s="1">
         <v>3215</v>
       </c>
@@ -4382,7 +4359,7 @@
       <c r="A18" s="7">
         <v>3</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="22">
         <v>50000</v>
       </c>
       <c r="C18" s="1">
@@ -4399,7 +4376,7 @@
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="23">
         <v>50000</v>
       </c>
       <c r="C19" s="1">
@@ -4416,7 +4393,7 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="22">
         <v>100000</v>
       </c>
       <c r="C20" s="1">
@@ -4433,7 +4410,7 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="23">
         <v>100000</v>
       </c>
       <c r="C21" s="1">
@@ -4447,10 +4424,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4462,7 +4442,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C18" sqref="C18:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4497,22 +4477,22 @@
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="9">
         <v>301239</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="9">
         <v>276334</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="9">
         <v>1777222</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="9">
         <v>1442161</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="9">
         <v>4183835</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="9">
         <v>3268229</v>
       </c>
     </row>
@@ -4520,22 +4500,22 @@
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="9">
         <v>200161</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="9">
         <v>181592</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="9">
         <v>1243713</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="9">
         <v>1067728</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="9">
         <v>2822698</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="9">
         <v>2422996</v>
       </c>
     </row>
@@ -4543,22 +4523,22 @@
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="9">
         <v>191792</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="9">
         <v>170351</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="9">
         <v>1250146</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="9">
         <v>1109614</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="9">
         <v>2872916</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="9">
         <v>2431061</v>
       </c>
     </row>
@@ -4573,21 +4553,21 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
@@ -4602,16 +4582,16 @@
       <c r="A18" s="5">
         <v>1</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="21">
         <v>10000</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="9">
         <v>301239</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="9">
         <v>200161</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="9">
         <v>191792</v>
       </c>
     </row>
@@ -4619,14 +4599,14 @@
       <c r="A19" s="5">
         <v>2</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="19">
+      <c r="B19" s="21"/>
+      <c r="C19" s="9">
         <v>276334</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="9">
         <v>181592</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="9">
         <v>170351</v>
       </c>
     </row>
@@ -4634,16 +4614,16 @@
       <c r="A20" s="5">
         <v>3</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <v>50000</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="9">
         <v>1777222</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="9">
         <v>1243713</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="9">
         <v>1250146</v>
       </c>
     </row>
@@ -4651,14 +4631,14 @@
       <c r="A21" s="5">
         <v>4</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="19">
+      <c r="B21" s="21"/>
+      <c r="C21" s="9">
         <v>1442161</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="9">
         <v>1067728</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="9">
         <v>1109614</v>
       </c>
     </row>
@@ -4666,16 +4646,16 @@
       <c r="A22" s="5">
         <v>5</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="21">
         <v>100000</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="9">
         <v>4183835</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="9">
         <v>2822698</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="9">
         <v>2872916</v>
       </c>
     </row>
@@ -4683,25 +4663,25 @@
       <c r="A23" s="5">
         <v>6</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="19">
+      <c r="B23" s="21"/>
+      <c r="C23" s="9">
         <v>3268229</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="9">
         <v>2422996</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="9">
         <v>2431061</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>